<commit_message>
Land Update Sun 08/16/2020
</commit_message>
<xml_diff>
--- a/Health/Data/NC_COVID-19/5.18.2020/ByRace&Ethnicity.xlsx
+++ b/Health/Data/NC_COVID-19/5.18.2020/ByRace&Ethnicity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okgem\Documents\NC_DataDashboard\NC_COVID-19\5.18.2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5896e1b568e196aa/Desktop/GitHub/DataDashboard_Windows/Health/Data/NC_COVID-19/5.18.2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2A7DCF-365C-42CE-A149-350E7901A704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6344ED70-2EE3-429C-9E42-73032CC36ACA}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="22500" windowHeight="14710" xr2:uid="{6344ED70-2EE3-429C-9E42-73032CC36ACA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,13 +668,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969AD96E-DBCC-404D-89E0-41A71E16FF6F}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -689,7 +689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -711,7 +711,7 @@
       </c>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -762,7 +762,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
@@ -796,7 +796,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -813,7 +813,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
@@ -835,7 +835,7 @@
       </c>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>12</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>13</v>
       </c>

</xml_diff>